<commit_message>
Cronograma Dev e Arte.
</commit_message>
<xml_diff>
--- a/Doc/Entregas Patricia/Cronograma.xlsx
+++ b/Doc/Entregas Patricia/Cronograma.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacao\WorkSpace\git\repositorio\PanGu\Doc\Entregas Patricia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JobFera\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="103">
   <si>
     <t>Área</t>
   </si>
@@ -146,76 +146,196 @@
     <t>Responsavel 10</t>
   </si>
   <si>
-    <t>Dev1 - Atividade 13</t>
-  </si>
-  <si>
-    <t>Dev1 - Atividade 14</t>
-  </si>
-  <si>
-    <t>Dev1 - Atividade 15</t>
-  </si>
-  <si>
-    <t>Dev1 - Atividade 16</t>
-  </si>
-  <si>
-    <t>Dev1 - Atividade 17</t>
-  </si>
-  <si>
-    <t>Dev1 - Atividade 18</t>
-  </si>
-  <si>
-    <t>Dev1 - Atividade 19</t>
-  </si>
-  <si>
-    <t>Dev1 - Atividade 20</t>
-  </si>
-  <si>
     <t>to do</t>
   </si>
   <si>
     <t>Data final planejada</t>
   </si>
   <si>
-    <t>Pesquisa de tecnologias</t>
-  </si>
-  <si>
-    <t>Protótipo do level editor 2D</t>
-  </si>
-  <si>
-    <t>Protótipo do sistema de save/load</t>
-  </si>
-  <si>
-    <t>Versão Alpha</t>
-  </si>
-  <si>
-    <t>Protótipo da HUD(interface) do game</t>
-  </si>
-  <si>
-    <t>Protótipo do cenário(player, inimigos e itens)</t>
-  </si>
-  <si>
-    <t>Integração de artes</t>
-  </si>
-  <si>
-    <t>Versão Beta</t>
-  </si>
-  <si>
-    <t>Inclusão de audio</t>
-  </si>
-  <si>
-    <t>Desenvolvimento dos protótipos</t>
-  </si>
-  <si>
-    <t>Correção de Bugs</t>
-  </si>
-  <si>
-    <t>Integração de assets finais(artes, sons)</t>
-  </si>
-  <si>
-    <t>Jogos completo com menu, level editor 2D, save/load de fases desenvolvidas, game plataforma 2D</t>
-  </si>
-  <si>
-    <t>Implementar animações</t>
+    <t>Fase 1 - Protótipos</t>
+  </si>
+  <si>
+    <t>Pesquisa de tecnologias para desenvolvimento(linguagem, engine, etc.)</t>
+  </si>
+  <si>
+    <t>Jefferson</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Fase 1.1 - Level Editor 2D</t>
+  </si>
+  <si>
+    <t>Pesquisa/Desenvolvimento do grid na tela</t>
+  </si>
+  <si>
+    <t>Pesquisa/Desenvolvimento do sistema de posicionamento de tiles</t>
+  </si>
+  <si>
+    <t>Testes e correções de bugs</t>
+  </si>
+  <si>
+    <t>Fase 1.2 - Sistema de Save/Load</t>
+  </si>
+  <si>
+    <t>Pesquisa do sistema de save/load</t>
+  </si>
+  <si>
+    <t>Definição de tecnologia(ScriptableObject, XML, JSON )</t>
+  </si>
+  <si>
+    <t>doing</t>
+  </si>
+  <si>
+    <t>Desenvolvimento do sistema de save/load</t>
+  </si>
+  <si>
+    <t>Fase 1.3 - Cenário</t>
+  </si>
+  <si>
+    <t>Inclusão: player, inimigo, item e background</t>
+  </si>
+  <si>
+    <t>Jefferson/Maiara</t>
+  </si>
+  <si>
+    <t>Desenvolvimento do cenário</t>
+  </si>
+  <si>
+    <t>Fase 1.4 - HUD</t>
+  </si>
+  <si>
+    <t>Inclusão: barra de itens e botões(apagar itens e salvar fase)</t>
+  </si>
+  <si>
+    <t>Fase 2 - Versão Beta</t>
+  </si>
+  <si>
+    <t>Fase 1 - Conceito e criação base</t>
+  </si>
+  <si>
+    <t>Discussão/definição temática de roteiro pelo grupo</t>
+  </si>
+  <si>
+    <t>Jefferson + grupo</t>
+  </si>
+  <si>
+    <t>Fase 1.1 - A protagonista</t>
+  </si>
+  <si>
+    <t>Brainstorm/definição sobre temática de cenário e assets</t>
+  </si>
+  <si>
+    <t>Jefferson/Renan/Michel</t>
+  </si>
+  <si>
+    <t>Pesquisa/Estudo de shape da personagem protagonista</t>
+  </si>
+  <si>
+    <t>Renan/Michel</t>
+  </si>
+  <si>
+    <t>Esboços/concepts do shape básico da personagem protagonista</t>
+  </si>
+  <si>
+    <t>Renan</t>
+  </si>
+  <si>
+    <t>Proposta de shape básico da personagem protagonista</t>
+  </si>
+  <si>
+    <t>desenho de sprites básicos de movimento</t>
+  </si>
+  <si>
+    <t>Digitalização e Arte finalização dos sprites básicos de movimento</t>
+  </si>
+  <si>
+    <t>Michel</t>
+  </si>
+  <si>
+    <t>Testes práticos de uso de sprites básicos de movimento</t>
+  </si>
+  <si>
+    <t>Michel/Jefferson</t>
+  </si>
+  <si>
+    <t>Período de correções de sprites de movimento</t>
+  </si>
+  <si>
+    <t>Fase 1.2 - Assets de cenário</t>
+  </si>
+  <si>
+    <t>Brainstorm/definição sobre temática de assets de cenário e inimigos</t>
+  </si>
+  <si>
+    <t>Pesquisa/Estudo de assets de cenários</t>
+  </si>
+  <si>
+    <t>Esboços/concepts de assets de cenários</t>
+  </si>
+  <si>
+    <t>Proposta de assets de cenários básicos</t>
+  </si>
+  <si>
+    <t>Digitalização e Arte finalização de assets de cenários</t>
+  </si>
+  <si>
+    <t>Testes práticos de assets de cenários</t>
+  </si>
+  <si>
+    <t>Período de correções de assets de cenários</t>
+  </si>
+  <si>
+    <t>Fase 1.3 - Inimigos nível 1</t>
+  </si>
+  <si>
+    <t>Pesquisa/Estudo de shape de inimigos nível 1</t>
+  </si>
+  <si>
+    <t>Esboços/concepts de 3 inimigos nível 1</t>
+  </si>
+  <si>
+    <t>Proposta de assets de inimigos nível1</t>
+  </si>
+  <si>
+    <t>Desenho de sprites básicos de movimento</t>
+  </si>
+  <si>
+    <t>Digitalização e Arte finalização de inimigos nível 1</t>
+  </si>
+  <si>
+    <t>Testes práticos de assets de inimigos nível 1</t>
+  </si>
+  <si>
+    <t>Período de correções de inimigos nível 1</t>
+  </si>
+  <si>
+    <t>Fase 1.4 - Cenário</t>
+  </si>
+  <si>
+    <t>Pesquisa/Estudo de cenários 2D para games plataforma</t>
+  </si>
+  <si>
+    <t>Esboços/concepts de cenário</t>
+  </si>
+  <si>
+    <t>Proposta de assets de cenário</t>
+  </si>
+  <si>
+    <t>Digitalização e Arte finalização do cenário</t>
+  </si>
+  <si>
+    <t>Testes práticos do cenário</t>
+  </si>
+  <si>
+    <t>Período de correções do cenário</t>
+  </si>
+  <si>
+    <t>Fase 2 - Aperfeiçoamento</t>
+  </si>
+  <si>
+    <t>Arte</t>
   </si>
 </sst>
 </file>
@@ -225,7 +345,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-416]d\-mmm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +357,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -256,7 +384,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -316,11 +444,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -336,6 +497,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,17 +788,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B34" sqref="A34:XFD34"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="89.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
@@ -672,11 +844,11 @@
         <v>42371</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G2" s="2"/>
       <c r="I2" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -694,7 +866,7 @@
         <v>42372</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G3" s="2"/>
       <c r="I3" s="5">
@@ -716,7 +888,7 @@
         <v>42373</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -735,7 +907,7 @@
         <v>42374</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -754,7 +926,7 @@
         <v>42375</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -773,7 +945,7 @@
         <v>42376</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -792,7 +964,7 @@
         <v>42377</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -811,7 +983,7 @@
         <v>42378</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -830,7 +1002,7 @@
         <v>42379</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -849,7 +1021,7 @@
         <v>42380</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -868,7 +1040,7 @@
         <v>42381</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -887,7 +1059,7 @@
         <v>42382</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G13" s="2"/>
     </row>
@@ -906,7 +1078,7 @@
         <v>42383</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G14" s="2"/>
     </row>
@@ -925,7 +1097,7 @@
         <v>42384</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G15" s="2"/>
     </row>
@@ -944,7 +1116,7 @@
         <v>42385</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -963,7 +1135,7 @@
         <v>42386</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G17" s="2"/>
     </row>
@@ -982,7 +1154,7 @@
         <v>42387</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G18" s="2"/>
     </row>
@@ -1001,7 +1173,7 @@
         <v>42388</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G19" s="2"/>
     </row>
@@ -1020,7 +1192,7 @@
         <v>42389</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G20" s="2"/>
     </row>
@@ -1039,7 +1211,7 @@
         <v>42390</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G21" s="2"/>
     </row>
@@ -1047,122 +1219,106 @@
       <c r="A22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="3">
-        <v>42390</v>
-      </c>
-      <c r="E22" s="3">
-        <v>42391</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D23" s="3">
-        <v>42391</v>
+        <v>42413</v>
       </c>
       <c r="E23" s="3">
-        <v>42392</v>
+        <v>42420</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="3">
-        <v>42392</v>
-      </c>
-      <c r="E24" s="3">
-        <v>42393</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B24" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D25" s="3">
-        <v>42393</v>
+        <v>42420</v>
       </c>
       <c r="E25" s="3">
-        <v>42394</v>
+        <v>42427</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D26" s="3">
-        <v>42394</v>
+        <v>42427</v>
       </c>
       <c r="E26" s="3">
-        <v>42395</v>
+        <v>42434</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D27" s="3">
-        <v>42395</v>
+        <v>42434</v>
       </c>
       <c r="E27" s="3">
-        <v>42396</v>
+        <v>42441</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="2" t="s">
-        <v>55</v>
+      <c r="B28" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
@@ -1173,285 +1329,834 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="3">
+        <v>42441</v>
+      </c>
+      <c r="E29" s="3">
+        <v>42448</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D30" s="3">
-        <v>42396</v>
+        <v>42448</v>
       </c>
       <c r="E30" s="3">
-        <v>42397</v>
+        <v>42455</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D31" s="3">
-        <v>42397</v>
+        <v>42455</v>
       </c>
       <c r="E31" s="3">
-        <v>42398</v>
+        <v>42462</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
-      <c r="B32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="3">
-        <v>42398</v>
-      </c>
-      <c r="E32" s="3">
-        <v>42399</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B32" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
-      <c r="B33" s="2" t="s">
-        <v>59</v>
+      <c r="B33" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D33" s="3">
-        <v>42399</v>
+        <v>42462</v>
       </c>
       <c r="E33" s="3">
-        <v>42400</v>
+        <v>42469</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="2" t="s">
-        <v>60</v>
+      <c r="B34" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D34" s="3">
-        <v>42400</v>
+        <v>42469</v>
       </c>
       <c r="E34" s="3">
-        <v>42401</v>
+        <v>42476</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="B35" s="2" t="s">
-        <v>61</v>
+      <c r="B35" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="D35" s="3">
-        <v>42401</v>
+        <v>42476</v>
       </c>
       <c r="E35" s="3">
-        <v>42402</v>
+        <v>42483</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="3">
-        <v>42402</v>
-      </c>
-      <c r="E36" s="3">
-        <v>42403</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B36" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="2" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="D37" s="3">
-        <v>42403</v>
+        <v>42483</v>
       </c>
       <c r="E37" s="3">
-        <v>42404</v>
+        <v>42490</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D38" s="3">
-        <v>42404</v>
+        <v>42490</v>
       </c>
       <c r="E38" s="3">
-        <v>42405</v>
+        <v>42497</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="3">
-        <v>42405</v>
-      </c>
-      <c r="E39" s="3">
-        <v>42406</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="3">
-        <v>42406</v>
-      </c>
-      <c r="E40" s="3">
-        <v>42407</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="A40" s="8"/>
+      <c r="B40" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="2" t="s">
+      <c r="A41" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="3">
+        <v>42441</v>
+      </c>
+      <c r="E42" s="3">
+        <v>42448</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="3">
-        <v>42407</v>
-      </c>
-      <c r="E41" s="3">
-        <v>42408</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" s="3">
-        <v>42408</v>
-      </c>
-      <c r="E42" s="3">
-        <v>42409</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D43" s="3">
-        <v>42409</v>
-      </c>
-      <c r="E43" s="3">
-        <v>42410</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="A43" s="14"/>
+      <c r="B43" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
       <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="3">
+        <v>42448</v>
+      </c>
+      <c r="E44" s="3">
+        <v>42448</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="3">
+        <v>42449</v>
+      </c>
+      <c r="E45" s="3">
+        <v>42453</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="3">
+        <v>42453</v>
+      </c>
+      <c r="E46" s="3">
+        <v>42459</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="3">
+        <v>42459</v>
+      </c>
+      <c r="E47" s="3">
+        <v>42463</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="3">
+        <v>42464</v>
+      </c>
+      <c r="E48" s="3">
+        <v>42471</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" s="3">
+        <v>42471</v>
+      </c>
+      <c r="E49" s="3">
+        <v>42476</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="3">
+        <v>42476</v>
+      </c>
+      <c r="E50" s="3">
+        <v>42477</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="3">
+        <v>42476</v>
+      </c>
+      <c r="E51" s="3">
+        <v>42480</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" s="3">
+        <v>42481</v>
+      </c>
+      <c r="E53" s="3">
+        <v>42483</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54" s="3">
+        <v>42483</v>
+      </c>
+      <c r="E54" s="3">
+        <v>42490</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="14"/>
+      <c r="B55" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="3">
+        <v>42485</v>
+      </c>
+      <c r="E55" s="3">
+        <v>42520</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D56" s="3">
+        <v>42485</v>
+      </c>
+      <c r="E56" s="3">
+        <v>42492</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57" s="3">
+        <v>42492</v>
+      </c>
+      <c r="E57" s="3">
+        <v>42497</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
+      <c r="B58" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="3">
+        <v>42497</v>
+      </c>
+      <c r="E58" s="3">
+        <v>42498</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59" s="3">
+        <v>42497</v>
+      </c>
+      <c r="E59" s="3">
+        <v>42504</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" s="3">
+        <v>42501</v>
+      </c>
+      <c r="E61" s="3">
+        <v>42508</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D62" s="3">
+        <v>42508</v>
+      </c>
+      <c r="E62" s="3">
+        <v>42515</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63" s="3">
+        <v>42513</v>
+      </c>
+      <c r="E63" s="3">
+        <v>42518</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D64" s="3">
+        <v>42518</v>
+      </c>
+      <c r="E64" s="3">
+        <v>42532</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="B65" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" s="3">
+        <v>42532</v>
+      </c>
+      <c r="E65" s="3">
+        <v>42539</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="B66" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" s="3">
+        <v>42539</v>
+      </c>
+      <c r="E66" s="3">
+        <v>42540</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
+      <c r="B67" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="3">
+        <v>42539</v>
+      </c>
+      <c r="E67" s="3">
+        <v>42546</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+      <c r="B68" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+      <c r="B69" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69" s="3">
+        <v>42543</v>
+      </c>
+      <c r="E69" s="3">
+        <v>42550</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
+      <c r="B70" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70" s="3">
+        <v>42550</v>
+      </c>
+      <c r="E70" s="3">
+        <v>42564</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D71" s="3">
+        <v>42555</v>
+      </c>
+      <c r="E71" s="3">
+        <v>42567</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
+      <c r="B72" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D72" s="3">
+        <v>42567</v>
+      </c>
+      <c r="E72" s="3">
+        <v>42574</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="7"/>
+      <c r="B73" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D73" s="3">
+        <v>42574</v>
+      </c>
+      <c r="E73" s="3">
+        <v>42575</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="7"/>
+      <c r="B74" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D74" s="3">
+        <v>42574</v>
+      </c>
+      <c r="E74" s="3">
+        <v>42581</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="7"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="8"/>
+      <c r="B76" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1"/>
-  <mergeCells count="2">
+  <mergeCells count="4">
+    <mergeCell ref="A60:A76"/>
     <mergeCell ref="A2:A21"/>
-    <mergeCell ref="A22:A43"/>
+    <mergeCell ref="A22:A40"/>
+    <mergeCell ref="A41:A59"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>